<commit_message>
wrote script to extract monthly data from weekly data
</commit_message>
<xml_diff>
--- a/Current_Data/New_data.xlsx
+++ b/Current_Data/New_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amirgirgis/Library/Containers/com.microsoft.Excel/Data/Desktop/College/PURA Award/Project/Current_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amirgirgis/Desktop/College/PURA Award/Project/Current_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCEAFCF-5FC5-3E40-A099-26A7066ADCAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E979849D-29F4-9D4C-BC22-98995ADB7788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33700" windowHeight="19800" xr2:uid="{F89DAAEF-60D4-7048-966D-D0EADBD8175A}"/>
   </bookViews>
@@ -3995,7 +3995,7 @@
   <dimension ref="A1:G2823"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4028,7 +4028,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C2" s="3">
         <v>11</v>
@@ -4046,7 +4046,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C3" s="3">
         <v>88</v>
@@ -4064,7 +4064,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -4082,7 +4082,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -4100,7 +4100,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -4118,7 +4118,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -4136,7 +4136,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -4154,7 +4154,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C9" s="3">
         <v>3</v>
@@ -4172,7 +4172,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C10" s="3">
         <v>7</v>
@@ -4190,7 +4190,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="4">
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C11" s="3">
         <v>7</v>

</xml_diff>